<commit_message>
new chnages in test data file
</commit_message>
<xml_diff>
--- a/Testdata/Userdata.xlsx
+++ b/Testdata/Userdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13080" windowHeight="3330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13080" windowHeight="3330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -140,10 +140,10 @@
     <t>Window Testing</t>
   </si>
   <si>
-    <t>Web Development_Pragna</t>
-  </si>
-  <si>
     <t>Username</t>
+  </si>
+  <si>
+    <t>Web Development</t>
   </si>
 </sst>
 </file>
@@ -489,7 +489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -501,7 +501,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>33</v>
@@ -576,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -624,7 +624,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
few more minor changes add in testdata
</commit_message>
<xml_diff>
--- a/Testdata/Userdata.xlsx
+++ b/Testdata/Userdata.xlsx
@@ -143,7 +143,7 @@
     <t>Username</t>
   </si>
   <si>
-    <t>Web Development</t>
+    <t>WEB DEVELOPMENT</t>
   </si>
 </sst>
 </file>
@@ -577,7 +577,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>